<commit_message>
Fix positioning issues with copy buttons and textboxes
Problem:
- Copy buttons had absolute positioning with bottom: 0
- This caused buttons to overlap with textboxes
- Buttons appeared above the top edge of their containers

Solution:
- Changed copy button positioning from bottom: 0 to bottom: -40px
- Added margin-bottom: 40px to all header containers
- This properly spaces the button below the label and above the textbox
- Maintains the original design intent while fixing overlap issues

Affected components:
- .snefuru-header303-db-mapping-header
- .snefuru-header303-header
- .snefuru-elementor-data-header
- .snefuru-copy-btn

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/210 sddx - pantheon table tenants - 1/210 sddx - pantheon table tenants - 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/210 sddx - pantheon table tenants - 1/210 sddx - pantheon table tenants - 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/210 sddx - pantheon table tenants - 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B448E5B-EC7F-914F-A52E-406F4BA5FEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EA1394-4515-3B44-864A-59BC41C635EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{800A12F4-B84A-EC41-88CA-9666E3C00132}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>description</t>
   </si>
@@ -453,7 +453,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,12 +518,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Add 3 denyeep column div areas to Image Freeway tab
- Created column container wrapper with flexbox layout
- Added 3 denyeep column divs with consistent styling:
  - Black 1px solid border
  - 10px padding
  - Flex: 1 with min-width: 420px
  - 15px gap between columns
- Each column includes:
  - Bold 16px "denyeep column div [1/2/3]" label
  - HR separator below the label
  - Empty content area for future additions
- Matches the exact style of denyeep columns in other tabs

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/210 sddx - pantheon table tenants - 1/210 sddx - pantheon table tenants - 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/210 sddx - pantheon table tenants - 1/210 sddx - pantheon table tenants - 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/210 sddx - pantheon table tenants - 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EA1394-4515-3B44-864A-59BC41C635EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA6FEB8-8BB8-BB4E-93F9-A26276C36103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{800A12F4-B84A-EC41-88CA-9666E3C00132}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
   <si>
     <t>description</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>open /driggsman?PARAMETER</t>
+  </si>
+  <si>
+    <t>///</t>
   </si>
 </sst>
 </file>
@@ -449,11 +452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70827F30-29D4-3049-AB31-D2A38108864F}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,8 +467,37 @@
     <col min="5" max="5" width="46.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -479,30 +511,51 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -510,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -518,25 +571,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>